<commit_message>
6/19/17 Its about time, but heres a working capture , woot
</commit_message>
<xml_diff>
--- a/JsDev/DD_POC_v2/productOwnerWorkRequests/Positive Flow-Non senior plan.xlsx
+++ b/JsDev/DD_POC_v2/productOwnerWorkRequests/Positive Flow-Non senior plan.xlsx
@@ -9,12 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="1050" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t xml:space="preserve">Scenario </t>
   </si>
@@ -272,6 +270,15 @@
   </si>
   <si>
     <t>Plan details should expand/collapse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use the URL server:3000/enroll    or   what ever URL is necessary that takes you to the similar page to how AWS DEV STARTS   </t>
+  </si>
+  <si>
+    <t>example : https://mot.deltadentalins.com/enroll/         or    https://dit3.deltadentalins.com/enroll   I think you get the example</t>
+  </si>
+  <si>
+    <t>Follow the instructions   .  ASK Questions.  I</t>
   </si>
 </sst>
 </file>
@@ -382,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -411,6 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -692,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,130 +748,108 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -871,15 +857,9 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="2">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -888,15 +868,9 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -904,89 +878,83 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C12" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="2">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2">
-        <v>9</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="7"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -995,13 +963,13 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1012,98 +980,104 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="2">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="3">
-        <v>201285</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="3"/>
       <c r="H21" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2">
+        <v>9</v>
+      </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="7"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="B23" s="3"/>
       <c r="C23" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1112,13 +1086,13 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1129,32 +1103,32 @@
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="2">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="G26" s="4"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1163,62 +1137,62 @@
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="2">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="4"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="2">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="E28" s="3">
+        <v>201285</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="2">
-        <v>7</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="B30" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C30" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1229,13 +1203,13 @@
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1246,16 +1220,16 @@
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
@@ -1263,16 +1237,16 @@
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="2">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
@@ -1280,13 +1254,13 @@
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -1297,30 +1271,30 @@
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3" t="s">
-        <v>58</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="2">
+        <v>7</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="E36" s="3"/>
-      <c r="F36" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -1329,15 +1303,15 @@
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="2">
-        <v>1</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -1346,13 +1320,13 @@
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -1363,15 +1337,15 @@
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -1380,13 +1354,13 @@
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -1397,15 +1371,15 @@
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -1413,29 +1387,31 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="3"/>
+      <c r="C42" s="2">
+        <v>13</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" s="3"/>
+      <c r="B43" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -1444,15 +1420,15 @@
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="2">
-        <v>2</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -1461,13 +1437,13 @@
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E45" s="14">
-        <v>43070</v>
+        <v>63</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -1478,15 +1454,15 @@
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F46" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -1495,12 +1471,14 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E47" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -1510,18 +1488,18 @@
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G48" s="3"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
@@ -1531,56 +1509,145 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C50" s="2">
         <v>1</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3" t="s">
-        <v>81</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="2">
+        <v>2</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="2">
+        <v>3</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="14">
+        <v>43070</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="2">
+        <v>4</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="2">
+        <v>5</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="2">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E18" r:id="rId1"/>
+    <hyperlink ref="E25" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>